<commit_message>
Data Update for 16-04-2020
</commit_message>
<xml_diff>
--- a/source-xlsx/16-04-2020.xlsx
+++ b/source-xlsx/16-04-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\covid19\source-xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1CBE8A-395A-4F6E-AE4D-BF0C193A5F48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A189802C-5F81-4C3D-8B50-D78398860D9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="154">
   <si>
     <t>division</t>
   </si>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="H147" sqref="H147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -885,7 +885,9 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -895,7 +897,9 @@
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -905,7 +909,9 @@
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -915,7 +921,9 @@
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -925,7 +933,9 @@
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -935,7 +945,9 @@
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -945,7 +957,9 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -955,7 +969,9 @@
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -965,7 +981,9 @@
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="4"/>
+      <c r="A11" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
@@ -975,7 +993,9 @@
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
@@ -985,7 +1005,9 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
@@ -995,7 +1017,9 @@
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1005,7 +1029,9 @@
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="5"/>
+      <c r="A15" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1027,7 +1053,9 @@
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="5"/>
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1037,7 +1065,9 @@
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="5"/>
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
@@ -1047,7 +1077,9 @@
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="5"/>
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1057,7 +1089,9 @@
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="5"/>
+      <c r="A20" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1067,7 +1101,9 @@
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="5"/>
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1077,7 +1113,9 @@
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="5"/>
+      <c r="A22" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1099,7 +1137,9 @@
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="5"/>
+      <c r="A24" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
@@ -1109,7 +1149,9 @@
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="5"/>
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>27</v>
       </c>
@@ -1119,7 +1161,9 @@
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="5"/>
+      <c r="A26" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>28</v>
       </c>
@@ -1141,7 +1185,9 @@
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="5"/>
+      <c r="A28" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1151,7 +1197,9 @@
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="5"/>
+      <c r="A29" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B29" s="2" t="s">
         <v>31</v>
       </c>
@@ -1161,7 +1209,9 @@
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="5"/>
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
@@ -1171,7 +1221,9 @@
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="5"/>
+      <c r="A31" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
@@ -1181,7 +1233,9 @@
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="5"/>
+      <c r="A32" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B32" s="2" t="s">
         <v>34</v>
       </c>
@@ -1191,7 +1245,9 @@
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="5"/>
+      <c r="A33" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B33" s="2" t="s">
         <v>35</v>
       </c>
@@ -1213,7 +1269,9 @@
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="5"/>
+      <c r="A35" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="B35" s="2" t="s">
         <v>37</v>
       </c>
@@ -1223,7 +1281,9 @@
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="5"/>
+      <c r="A36" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="B36" s="2" t="s">
         <v>38</v>
       </c>
@@ -1245,7 +1305,9 @@
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="5"/>
+      <c r="A38" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B38" s="2" t="s">
         <v>40</v>
       </c>
@@ -1255,7 +1317,9 @@
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="5"/>
+      <c r="A39" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B39" s="2" t="s">
         <v>41</v>
       </c>
@@ -1265,7 +1329,9 @@
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="5"/>
+      <c r="A40" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B40" s="2" t="s">
         <v>15</v>
       </c>
@@ -1287,7 +1353,9 @@
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="5"/>
+      <c r="A42" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="B42" s="2" t="s">
         <v>43</v>
       </c>
@@ -1297,7 +1365,9 @@
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="5"/>
+      <c r="A43" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="B43" s="2" t="s">
         <v>44</v>
       </c>
@@ -1307,7 +1377,9 @@
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="5"/>
+      <c r="A44" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="B44" s="2" t="s">
         <v>45</v>
       </c>
@@ -1317,7 +1389,9 @@
       <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="5"/>
+      <c r="A45" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="B45" s="2" t="s">
         <v>46</v>
       </c>

</xml_diff>